<commit_message>
added unison to the list
</commit_message>
<xml_diff>
--- a/softwaresToBeInstalled.xlsx
+++ b/softwaresToBeInstalled.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>serial</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>Record my desktop</t>
+  </si>
+  <si>
+    <t>Unison</t>
+  </si>
+  <si>
+    <t>For syncing folders.</t>
   </si>
 </sst>
 </file>
@@ -207,18 +213,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:C27"/>
+  <dimension ref="A3:C28"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A23" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A28" activeCellId="0" pane="topLeft" sqref="A28"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C17" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C29" activeCellId="0" pane="topLeft" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2039215686275"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="143.447058823529"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="89.9450980392157"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.8901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.74901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="144.043137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="90.3176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.0666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.7843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
@@ -409,6 +415,17 @@
       </c>
       <c r="B27" s="0" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
+      <c r="A28" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -434,7 +451,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.74901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.7843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -459,7 +476,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.74901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.7843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>